<commit_message>
convert latest mex files to xlsx.  orphan id handling in clean_segments.
</commit_message>
<xml_diff>
--- a/data/coded_segments/md_3_2.xlsx
+++ b/data/coded_segments/md_3_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76FC17E2-21D7-B947-88BE-FE501164E6B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFBA5AB5-0DA5-C247-ABAE-37E83E831C27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1211,20 +1211,6 @@
     <t>7/10/18 11:44:00</t>
   </si>
   <si>
-    <t>1: 2895</t>
-  </si>
-  <si>
-    <t>1: 2935</t>
-  </si>
-  <si>
-    <t>Acinetobacter  
-baumannii  
-Osteomyelitis</t>
-  </si>
-  <si>
-    <t>7/10/18 11:45:00</t>
-  </si>
-  <si>
     <t>2: 1650</t>
   </si>
   <si>
@@ -2011,6 +1997,19 @@
   </si>
   <si>
     <t>11/8/18 14:20:00</t>
+  </si>
+  <si>
+    <t>1: 2895</t>
+  </si>
+  <si>
+    <t>1: 2919</t>
+  </si>
+  <si>
+    <t>Acinetobacter  
+baumannii</t>
+  </si>
+  <si>
+    <t>11/19/18 13:23:00</t>
   </si>
 </sst>
 </file>
@@ -7574,7 +7573,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>13</v>
       </c>
@@ -7603,10 +7602,10 @@
         <v>396</v>
       </c>
       <c r="J125" s="3">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="K125" s="4">
-        <v>0.23549300000000001</v>
+        <v>6.6420999999999994E-2</v>
       </c>
       <c r="L125" s="1" t="s">
         <v>20</v>
@@ -7626,34 +7625,34 @@
         <v>14</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H126" s="3">
         <v>0</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="J126" s="3">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K126" s="4">
-        <v>6.6420999999999994E-2</v>
+        <v>2.4799000000000002E-2</v>
       </c>
       <c r="L126" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7667,34 +7666,34 @@
         <v>14</v>
       </c>
       <c r="D127" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F127" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G127" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="H127" s="3">
         <v>0</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>405</v>
+        <v>174</v>
       </c>
       <c r="J127" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K127" s="4">
-        <v>2.4799000000000002E-2</v>
+        <v>4.9597000000000002E-2</v>
       </c>
       <c r="L127" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="128" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7708,34 +7707,34 @@
         <v>14</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H128" s="3">
         <v>0</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
       <c r="J128" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K128" s="4">
-        <v>4.9597000000000002E-2</v>
+        <v>6.1996000000000002E-2</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="129" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7749,34 +7748,34 @@
         <v>14</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="H129" s="3">
+        <v>0</v>
+      </c>
+      <c r="I129" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G129" s="1" t="s">
+      <c r="J129" s="3">
+        <v>22</v>
+      </c>
+      <c r="K129" s="4">
+        <v>0.27278400000000003</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M129" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="H129" s="3">
-        <v>0</v>
-      </c>
-      <c r="I129" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J129" s="3">
-        <v>5</v>
-      </c>
-      <c r="K129" s="4">
-        <v>6.1996000000000002E-2</v>
-      </c>
-      <c r="L129" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M129" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="130" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7790,10 +7789,10 @@
         <v>14</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>410</v>
@@ -7808,16 +7807,16 @@
         <v>412</v>
       </c>
       <c r="J130" s="3">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K130" s="4">
-        <v>0.27278400000000003</v>
+        <v>0.12399300000000001</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="131" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7831,34 +7830,34 @@
         <v>14</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="F131" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H131" s="3">
+        <v>0</v>
+      </c>
+      <c r="I131" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="J131" s="3">
+        <v>21</v>
+      </c>
+      <c r="K131" s="4">
+        <v>0.260384</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M131" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="H131" s="3">
-        <v>0</v>
-      </c>
-      <c r="I131" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="J131" s="3">
-        <v>10</v>
-      </c>
-      <c r="K131" s="4">
-        <v>0.12399300000000001</v>
-      </c>
-      <c r="L131" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M131" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="132" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7872,16 +7871,16 @@
         <v>14</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H132" s="3">
         <v>0</v>
@@ -7890,16 +7889,16 @@
         <v>418</v>
       </c>
       <c r="J132" s="3">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="K132" s="4">
-        <v>0.260384</v>
+        <v>9.9194000000000004E-2</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M132" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7913,34 +7912,34 @@
         <v>14</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>182</v>
+        <v>316</v>
       </c>
       <c r="F133" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="H133" s="3">
+        <v>0</v>
+      </c>
+      <c r="I133" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="H133" s="3">
-        <v>0</v>
-      </c>
-      <c r="I133" s="2" t="s">
-        <v>422</v>
-      </c>
       <c r="J133" s="3">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="K133" s="4">
-        <v>9.9194000000000004E-2</v>
+        <v>0.23558599999999999</v>
       </c>
       <c r="L133" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M133" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="134" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7954,10 +7953,10 @@
         <v>14</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>316</v>
+        <v>422</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>423</v>
@@ -7972,16 +7971,16 @@
         <v>425</v>
       </c>
       <c r="J134" s="3">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K134" s="4">
-        <v>0.23558599999999999</v>
+        <v>0.17358999999999999</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M134" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="135" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7995,22 +7994,22 @@
         <v>14</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>426</v>
+        <v>39</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H135" s="3">
         <v>0</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="J135" s="3">
         <v>14</v>
@@ -8022,7 +8021,7 @@
         <v>20</v>
       </c>
       <c r="M135" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="136" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8036,10 +8035,10 @@
         <v>14</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>402</v>
+        <v>426</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>39</v>
+        <v>302</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>427</v>
@@ -8054,16 +8053,16 @@
         <v>429</v>
       </c>
       <c r="J136" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K136" s="4">
-        <v>0.17358999999999999</v>
+        <v>5.5689000000000002E-2</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M136" s="1" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
     </row>
     <row r="137" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8077,34 +8076,34 @@
         <v>14</v>
       </c>
       <c r="D137" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="H137" s="3">
+        <v>0</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="J137" s="3">
+        <v>5</v>
+      </c>
+      <c r="K137" s="4">
+        <v>2.7844000000000001E-2</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M137" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="H137" s="3">
-        <v>0</v>
-      </c>
-      <c r="I137" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="J137" s="3">
-        <v>10</v>
-      </c>
-      <c r="K137" s="4">
-        <v>5.5689000000000002E-2</v>
-      </c>
-      <c r="L137" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M137" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="138" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8118,34 +8117,34 @@
         <v>14</v>
       </c>
       <c r="D138" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H138" s="3">
+        <v>0</v>
+      </c>
+      <c r="I138" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J138" s="3">
+        <v>4</v>
+      </c>
+      <c r="K138" s="4">
+        <v>2.2275E-2</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M138" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="H138" s="3">
-        <v>0</v>
-      </c>
-      <c r="I138" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="J138" s="3">
-        <v>5</v>
-      </c>
-      <c r="K138" s="4">
-        <v>2.7844000000000001E-2</v>
-      </c>
-      <c r="L138" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8159,34 +8158,34 @@
         <v>14</v>
       </c>
       <c r="D139" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H139" s="3">
+        <v>0</v>
+      </c>
+      <c r="I139" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J139" s="3">
+        <v>2</v>
+      </c>
+      <c r="K139" s="4">
+        <v>1.1138E-2</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M139" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="H139" s="3">
-        <v>0</v>
-      </c>
-      <c r="I139" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="J139" s="3">
-        <v>4</v>
-      </c>
-      <c r="K139" s="4">
-        <v>2.2275E-2</v>
-      </c>
-      <c r="L139" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M139" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8200,34 +8199,34 @@
         <v>14</v>
       </c>
       <c r="D140" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H140" s="3">
+        <v>0</v>
+      </c>
+      <c r="I140" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J140" s="3">
+        <v>3</v>
+      </c>
+      <c r="K140" s="4">
+        <v>1.6707E-2</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M140" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="H140" s="3">
-        <v>0</v>
-      </c>
-      <c r="I140" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J140" s="3">
-        <v>2</v>
-      </c>
-      <c r="K140" s="4">
-        <v>1.1138E-2</v>
-      </c>
-      <c r="L140" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M140" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="141" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8241,34 +8240,34 @@
         <v>14</v>
       </c>
       <c r="D141" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H141" s="3">
+        <v>0</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="J141" s="3">
+        <v>8</v>
+      </c>
+      <c r="K141" s="4">
+        <v>4.4551E-2</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M141" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="H141" s="3">
-        <v>0</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J141" s="3">
-        <v>3</v>
-      </c>
-      <c r="K141" s="4">
-        <v>1.6707E-2</v>
-      </c>
-      <c r="L141" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M141" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="142" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8282,78 +8281,78 @@
         <v>14</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H142" s="3">
+        <v>0</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J142" s="3">
+        <v>5</v>
+      </c>
+      <c r="K142" s="4">
+        <v>2.7844000000000001E-2</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M142" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="E142" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="G142" s="1" t="s">
+    </row>
+    <row r="143" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A143" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="H142" s="3">
-        <v>0</v>
-      </c>
-      <c r="I142" s="2" t="s">
+      <c r="G143" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="J142" s="3">
-        <v>8</v>
-      </c>
-      <c r="K142" s="4">
-        <v>4.4551E-2</v>
-      </c>
-      <c r="L142" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M142" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D143" s="2" t="s">
+      <c r="H143" s="3">
+        <v>0</v>
+      </c>
+      <c r="I143" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="J143" s="3">
+        <v>16</v>
+      </c>
+      <c r="K143" s="4">
+        <v>8.9102000000000001E-2</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M143" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="E143" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H143" s="3">
-        <v>0</v>
-      </c>
-      <c r="I143" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J143" s="3">
-        <v>5</v>
-      </c>
-      <c r="K143" s="4">
-        <v>2.7844000000000001E-2</v>
-      </c>
-      <c r="L143" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M143" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>13</v>
       </c>
@@ -8364,34 +8363,34 @@
         <v>14</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F144" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G144" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="G144" s="1" t="s">
+      <c r="H144" s="3">
+        <v>0</v>
+      </c>
+      <c r="I144" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="H144" s="3">
-        <v>0</v>
-      </c>
-      <c r="I144" s="2" t="s">
+      <c r="J144" s="3">
+        <v>10</v>
+      </c>
+      <c r="K144" s="4">
+        <v>5.5689000000000002E-2</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M144" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="J144" s="3">
-        <v>16</v>
-      </c>
-      <c r="K144" s="4">
-        <v>8.9102000000000001E-2</v>
-      </c>
-      <c r="L144" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M144" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8405,7 +8404,7 @@
         <v>14</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>26</v>
@@ -8423,16 +8422,16 @@
         <v>453</v>
       </c>
       <c r="J145" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K145" s="4">
-        <v>5.5689000000000002E-2</v>
+        <v>3.3412999999999998E-2</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="146" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8446,10 +8445,10 @@
         <v>14</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>26</v>
+        <v>454</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>455</v>
@@ -8464,16 +8463,16 @@
         <v>457</v>
       </c>
       <c r="J146" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K146" s="4">
-        <v>3.3412999999999998E-2</v>
+        <v>2.7844000000000001E-2</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="147" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8487,37 +8486,37 @@
         <v>14</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E147" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F147" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="G147" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="H147" s="3">
+        <v>0</v>
+      </c>
+      <c r="I147" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="H147" s="3">
-        <v>0</v>
-      </c>
-      <c r="I147" s="2" t="s">
+      <c r="J147" s="3">
+        <v>12</v>
+      </c>
+      <c r="K147" s="4">
+        <v>6.6825999999999997E-2</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M147" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="J147" s="3">
-        <v>5</v>
-      </c>
-      <c r="K147" s="4">
-        <v>2.7844000000000001E-2</v>
-      </c>
-      <c r="L147" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M147" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>13</v>
       </c>
@@ -8528,10 +8527,10 @@
         <v>14</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>462</v>
@@ -8546,57 +8545,57 @@
         <v>464</v>
       </c>
       <c r="J148" s="3">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="K148" s="4">
-        <v>6.6825999999999997E-2</v>
+        <v>0.122515</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M148" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F149" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A149" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F149" s="1" t="s">
+      <c r="G149" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="H149" s="3">
+        <v>0</v>
+      </c>
+      <c r="I149" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="H149" s="3">
-        <v>0</v>
-      </c>
-      <c r="I149" s="2" t="s">
-        <v>468</v>
-      </c>
       <c r="J149" s="3">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="K149" s="4">
-        <v>0.122515</v>
+        <v>2.7844000000000001E-2</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M149" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8610,34 +8609,34 @@
         <v>14</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>430</v>
+        <v>468</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>324</v>
+        <v>49</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="G150" s="1" t="s">
+      <c r="H150" s="3">
+        <v>0</v>
+      </c>
+      <c r="I150" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="H150" s="3">
-        <v>0</v>
-      </c>
-      <c r="I150" s="2" t="s">
+      <c r="J150" s="3">
+        <v>4</v>
+      </c>
+      <c r="K150" s="4">
+        <v>9.6690000000000005E-3</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M150" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="J150" s="3">
-        <v>5</v>
-      </c>
-      <c r="K150" s="4">
-        <v>2.7844000000000001E-2</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M150" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8654,31 +8653,31 @@
         <v>472</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>49</v>
+        <v>473</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>67</v>
+        <v>474</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="H151" s="3">
         <v>0</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="J151" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K151" s="4">
-        <v>9.6690000000000005E-3</v>
+        <v>1.4418E-2</v>
       </c>
       <c r="L151" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="152" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8692,34 +8691,34 @@
         <v>14</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>477</v>
+        <v>49</v>
       </c>
       <c r="F152" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G152" s="1" t="s">
+      <c r="H152" s="3">
+        <v>0</v>
+      </c>
+      <c r="I152" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="H152" s="3">
-        <v>0</v>
-      </c>
-      <c r="I152" s="2" t="s">
+      <c r="J152" s="3">
+        <v>20</v>
+      </c>
+      <c r="K152" s="4">
+        <v>0.17413999999999999</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M152" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="J152" s="3">
-        <v>6</v>
-      </c>
-      <c r="K152" s="4">
-        <v>1.4418E-2</v>
-      </c>
-      <c r="L152" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M152" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="153" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8736,31 +8735,31 @@
         <v>481</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>49</v>
+        <v>260</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>67</v>
+        <v>482</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H153" s="3">
         <v>0</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="J153" s="3">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K153" s="4">
-        <v>0.17413999999999999</v>
+        <v>6.0962000000000002E-2</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M153" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="154" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8774,13 +8773,13 @@
         <v>14</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>260</v>
+        <v>49</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>486</v>
+        <v>60</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>487</v>
@@ -8795,13 +8794,13 @@
         <v>11</v>
       </c>
       <c r="K154" s="4">
-        <v>6.0962000000000002E-2</v>
+        <v>1.8762000000000001E-2</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M154" s="1" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="155" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8815,13 +8814,13 @@
         <v>14</v>
       </c>
       <c r="D155" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F155" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>491</v>
@@ -8833,16 +8832,16 @@
         <v>492</v>
       </c>
       <c r="J155" s="3">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K155" s="4">
-        <v>1.8762000000000001E-2</v>
+        <v>1.3291000000000001E-2</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M155" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="156" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8856,34 +8855,34 @@
         <v>14</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>260</v>
+        <v>49</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>494</v>
+        <v>67</v>
       </c>
       <c r="G156" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H156" s="3">
+        <v>0</v>
+      </c>
+      <c r="I156" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="H156" s="3">
-        <v>0</v>
-      </c>
-      <c r="I156" s="2" t="s">
+      <c r="J156" s="3">
+        <v>9</v>
+      </c>
+      <c r="K156" s="4">
+        <v>1.8384999999999999E-2</v>
+      </c>
+      <c r="L156" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M156" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="J156" s="3">
-        <v>3</v>
-      </c>
-      <c r="K156" s="4">
-        <v>1.3291000000000001E-2</v>
-      </c>
-      <c r="L156" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M156" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8897,34 +8896,34 @@
         <v>14</v>
       </c>
       <c r="D157" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F157" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="E157" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G157" s="1" t="s">
-        <v>68</v>
+        <v>499</v>
       </c>
       <c r="H157" s="3">
         <v>0</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="J157" s="3">
         <v>9</v>
       </c>
       <c r="K157" s="4">
-        <v>1.8384999999999999E-2</v>
+        <v>5.5174000000000001E-2</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M157" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="158" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8938,10 +8937,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>502</v>
@@ -8956,16 +8955,16 @@
         <v>504</v>
       </c>
       <c r="J158" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K158" s="4">
-        <v>5.5174000000000001E-2</v>
+        <v>2.4521999999999999E-2</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M158" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="159" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -8979,34 +8978,34 @@
         <v>14</v>
       </c>
       <c r="D159" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="H159" s="3">
+        <v>0</v>
+      </c>
+      <c r="I159" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="J159" s="3">
+        <v>2</v>
+      </c>
+      <c r="K159" s="4">
+        <v>1.2260999999999999E-2</v>
+      </c>
+      <c r="L159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M159" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="H159" s="3">
-        <v>0</v>
-      </c>
-      <c r="I159" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="J159" s="3">
-        <v>4</v>
-      </c>
-      <c r="K159" s="4">
-        <v>2.4521999999999999E-2</v>
-      </c>
-      <c r="L159" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M159" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="160" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9020,34 +9019,34 @@
         <v>14</v>
       </c>
       <c r="D160" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0</v>
+      </c>
+      <c r="I160" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="J160" s="3">
+        <v>3</v>
+      </c>
+      <c r="K160" s="4">
+        <v>1.8391000000000001E-2</v>
+      </c>
+      <c r="L160" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M160" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="H160" s="3">
-        <v>0</v>
-      </c>
-      <c r="I160" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="J160" s="3">
-        <v>2</v>
-      </c>
-      <c r="K160" s="4">
-        <v>1.2260999999999999E-2</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M160" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="161" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9061,34 +9060,34 @@
         <v>14</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F161" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="H161" s="3">
+        <v>0</v>
+      </c>
+      <c r="I161" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="G161" s="1" t="s">
+      <c r="J161" s="3">
+        <v>16</v>
+      </c>
+      <c r="K161" s="4">
+        <v>9.8086999999999994E-2</v>
+      </c>
+      <c r="L161" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M161" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="H161" s="3">
-        <v>0</v>
-      </c>
-      <c r="I161" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="J161" s="3">
-        <v>3</v>
-      </c>
-      <c r="K161" s="4">
-        <v>1.8391000000000001E-2</v>
-      </c>
-      <c r="L161" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M161" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="162" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9102,10 +9101,10 @@
         <v>14</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>513</v>
@@ -9120,10 +9119,10 @@
         <v>515</v>
       </c>
       <c r="J162" s="3">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K162" s="4">
-        <v>9.8086999999999994E-2</v>
+        <v>5.5174000000000001E-2</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>20</v>
@@ -9143,10 +9142,10 @@
         <v>14</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>517</v>
@@ -9161,16 +9160,16 @@
         <v>519</v>
       </c>
       <c r="J163" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K163" s="4">
-        <v>5.5174000000000001E-2</v>
+        <v>2.4521999999999999E-2</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M163" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="164" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9184,22 +9183,22 @@
         <v>14</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="H164" s="3">
         <v>0</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J164" s="3">
         <v>4</v>
@@ -9211,7 +9210,7 @@
         <v>20</v>
       </c>
       <c r="M164" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="165" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9225,34 +9224,34 @@
         <v>14</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="H165" s="3">
         <v>0</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="J165" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K165" s="4">
-        <v>2.4521999999999999E-2</v>
+        <v>5.5174000000000001E-2</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M165" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="166" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9266,34 +9265,34 @@
         <v>14</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="H166" s="3">
         <v>0</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="J166" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K166" s="4">
-        <v>5.5174000000000001E-2</v>
+        <v>6.1304999999999998E-2</v>
       </c>
       <c r="L166" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="167" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9307,22 +9306,22 @@
         <v>14</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="H167" s="3">
         <v>0</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J167" s="3">
         <v>10</v>
@@ -9334,7 +9333,7 @@
         <v>20</v>
       </c>
       <c r="M167" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="168" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9348,34 +9347,34 @@
         <v>14</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>524</v>
+        <v>230</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H168" s="3">
         <v>0</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="J168" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K168" s="4">
-        <v>6.1304999999999998E-2</v>
+        <v>2.4521999999999999E-2</v>
       </c>
       <c r="L168" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9389,22 +9388,22 @@
         <v>14</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>230</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="H169" s="3">
         <v>0</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J169" s="3">
         <v>4</v>
@@ -9416,7 +9415,7 @@
         <v>20</v>
       </c>
       <c r="M169" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="170" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9430,34 +9429,34 @@
         <v>14</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>230</v>
+        <v>524</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H170" s="3">
         <v>0</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="J170" s="3">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K170" s="4">
-        <v>2.4521999999999999E-2</v>
+        <v>6.7434999999999995E-2</v>
       </c>
       <c r="L170" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M170" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="171" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9471,22 +9470,22 @@
         <v>14</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H171" s="3">
         <v>0</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J171" s="3">
         <v>11</v>
@@ -9498,7 +9497,7 @@
         <v>20</v>
       </c>
       <c r="M171" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="172" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9512,34 +9511,34 @@
         <v>14</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="F172" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G172" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="G172" s="1" t="s">
-        <v>529</v>
-      </c>
       <c r="H172" s="3">
         <v>0</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="J172" s="3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K172" s="4">
-        <v>6.7434999999999995E-2</v>
+        <v>2.4521999999999999E-2</v>
       </c>
       <c r="L172" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M172" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="173" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9553,22 +9552,22 @@
         <v>14</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="H173" s="3">
         <v>0</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J173" s="3">
         <v>4</v>
@@ -9580,7 +9579,7 @@
         <v>20</v>
       </c>
       <c r="M173" s="1" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
     </row>
     <row r="174" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9594,34 +9593,34 @@
         <v>14</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F174" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G174" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G174" s="1" t="s">
+      <c r="H174" s="3">
+        <v>0</v>
+      </c>
+      <c r="I174" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="H174" s="3">
-        <v>0</v>
-      </c>
-      <c r="I174" s="2" t="s">
-        <v>523</v>
-      </c>
       <c r="J174" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K174" s="4">
-        <v>2.4521999999999999E-2</v>
+        <v>4.9043999999999997E-2</v>
       </c>
       <c r="L174" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M174" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="175" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9635,22 +9634,22 @@
         <v>14</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="H175" s="3">
         <v>0</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="J175" s="3">
         <v>8</v>
@@ -9662,7 +9661,7 @@
         <v>20</v>
       </c>
       <c r="M175" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="176" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9676,34 +9675,34 @@
         <v>14</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="F176" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="H176" s="3">
+        <v>0</v>
+      </c>
+      <c r="I176" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="G176" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="H176" s="3">
-        <v>0</v>
-      </c>
-      <c r="I176" s="2" t="s">
-        <v>536</v>
-      </c>
       <c r="J176" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K176" s="4">
-        <v>4.9043999999999997E-2</v>
+        <v>6.13E-3</v>
       </c>
       <c r="L176" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M176" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="177" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9717,22 +9716,22 @@
         <v>14</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="H177" s="3">
         <v>0</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="J177" s="3">
         <v>1</v>
@@ -9744,7 +9743,7 @@
         <v>20</v>
       </c>
       <c r="M177" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9758,34 +9757,34 @@
         <v>14</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H178" s="3">
         <v>0</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>538</v>
+        <v>185</v>
       </c>
       <c r="J178" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K178" s="4">
-        <v>6.13E-3</v>
+        <v>2.4521999999999999E-2</v>
       </c>
       <c r="L178" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M178" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="179" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9799,34 +9798,34 @@
         <v>14</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>182</v>
+        <v>316</v>
       </c>
       <c r="F179" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="H179" s="3">
+        <v>0</v>
+      </c>
+      <c r="I179" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="G179" s="1" t="s">
+      <c r="J179" s="3">
+        <v>12</v>
+      </c>
+      <c r="K179" s="4">
+        <v>7.3565000000000005E-2</v>
+      </c>
+      <c r="L179" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M179" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="H179" s="3">
-        <v>0</v>
-      </c>
-      <c r="I179" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J179" s="3">
-        <v>4</v>
-      </c>
-      <c r="K179" s="4">
-        <v>2.4521999999999999E-2</v>
-      </c>
-      <c r="L179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M179" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="180" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9840,10 +9839,10 @@
         <v>14</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>316</v>
+        <v>233</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>541</v>
@@ -9858,16 +9857,16 @@
         <v>543</v>
       </c>
       <c r="J180" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K180" s="4">
-        <v>7.3565000000000005E-2</v>
+        <v>5.5174000000000001E-2</v>
       </c>
       <c r="L180" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M180" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="181" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9881,34 +9880,34 @@
         <v>14</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>501</v>
+        <v>544</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>233</v>
+        <v>49</v>
       </c>
       <c r="F181" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H181" s="3">
+        <v>0</v>
+      </c>
+      <c r="I181" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="G181" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="H181" s="3">
-        <v>0</v>
-      </c>
-      <c r="I181" s="2" t="s">
-        <v>547</v>
-      </c>
       <c r="J181" s="3">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K181" s="4">
-        <v>5.5174000000000001E-2</v>
+        <v>5.6862999999999997E-2</v>
       </c>
       <c r="L181" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M181" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="182" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9922,16 +9921,16 @@
         <v>14</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>67</v>
+        <v>547</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>195</v>
+        <v>548</v>
       </c>
       <c r="H182" s="3">
         <v>0</v>
@@ -9940,16 +9939,16 @@
         <v>549</v>
       </c>
       <c r="J182" s="3">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="K182" s="4">
-        <v>5.6862999999999997E-2</v>
+        <v>2.8229000000000001E-2</v>
       </c>
       <c r="L182" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M182" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="183" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -9966,7 +9965,7 @@
         <v>550</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>551</v>
@@ -9981,16 +9980,16 @@
         <v>553</v>
       </c>
       <c r="J183" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K183" s="4">
-        <v>2.8229000000000001E-2</v>
+        <v>1.0127000000000001E-2</v>
       </c>
       <c r="L183" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M183" s="1" t="s">
-        <v>544</v>
+        <v>554</v>
       </c>
     </row>
     <row r="184" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10004,10 +10003,10 @@
         <v>14</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>555</v>
@@ -10019,83 +10018,83 @@
         <v>0</v>
       </c>
       <c r="I184" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J184" s="3">
+        <v>3</v>
+      </c>
+      <c r="K184" s="4">
+        <v>1.519E-2</v>
+      </c>
+      <c r="L184" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M184" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A185" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F185" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="J184" s="3">
-        <v>2</v>
-      </c>
-      <c r="K184" s="4">
-        <v>1.0127000000000001E-2</v>
-      </c>
-      <c r="L184" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M184" s="1" t="s">
+      <c r="G185" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="H185" s="3">
+        <v>0</v>
+      </c>
+      <c r="I185" s="2" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="185" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A185" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F185" s="1" t="s">
+      <c r="J185" s="3">
+        <v>34</v>
+      </c>
+      <c r="K185" s="4">
+        <v>0.172152</v>
+      </c>
+      <c r="L185" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M185" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="G185" s="1" t="s">
+    </row>
+    <row r="186" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A186" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F186" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="H185" s="3">
-        <v>0</v>
-      </c>
-      <c r="I185" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J185" s="3">
-        <v>3</v>
-      </c>
-      <c r="K185" s="4">
-        <v>1.519E-2</v>
-      </c>
-      <c r="L185" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M185" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A186" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F186" s="1" t="s">
+      <c r="G186" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="G186" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="H186" s="3">
         <v>0</v>
@@ -10104,16 +10103,16 @@
         <v>562</v>
       </c>
       <c r="J186" s="3">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="K186" s="4">
-        <v>0.172152</v>
+        <v>2.5316000000000002E-2</v>
       </c>
       <c r="L186" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M186" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="187" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10127,10 +10126,10 @@
         <v>14</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>39</v>
+        <v>563</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>564</v>
@@ -10145,16 +10144,16 @@
         <v>566</v>
       </c>
       <c r="J187" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K187" s="4">
-        <v>2.5316000000000002E-2</v>
+        <v>1.0127000000000001E-2</v>
       </c>
       <c r="L187" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M187" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="188" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10168,34 +10167,34 @@
         <v>14</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E188" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F188" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="F188" s="1" t="s">
+      <c r="G188" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="G188" s="1" t="s">
+      <c r="H188" s="3">
+        <v>0</v>
+      </c>
+      <c r="I188" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="H188" s="3">
-        <v>0</v>
-      </c>
-      <c r="I188" s="2" t="s">
-        <v>570</v>
-      </c>
       <c r="J188" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K188" s="4">
-        <v>1.0127000000000001E-2</v>
+        <v>3.5443000000000002E-2</v>
       </c>
       <c r="L188" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M188" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="189" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10209,34 +10208,34 @@
         <v>14</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F189" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="H189" s="3">
+        <v>0</v>
+      </c>
+      <c r="I189" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="G189" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="H189" s="3">
-        <v>0</v>
-      </c>
-      <c r="I189" s="2" t="s">
-        <v>573</v>
-      </c>
       <c r="J189" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K189" s="4">
-        <v>3.5443000000000002E-2</v>
+        <v>2.0253E-2</v>
       </c>
       <c r="L189" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M189" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="190" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10250,34 +10249,34 @@
         <v>14</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>574</v>
+        <v>299</v>
       </c>
       <c r="H190" s="3">
         <v>0</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>575</v>
+        <v>29</v>
       </c>
       <c r="J190" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K190" s="4">
-        <v>2.0253E-2</v>
+        <v>2.5316000000000002E-2</v>
       </c>
       <c r="L190" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M190" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="191" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10291,34 +10290,34 @@
         <v>14</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>391</v>
+        <v>572</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>299</v>
+        <v>573</v>
       </c>
       <c r="H191" s="3">
         <v>0</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>29</v>
+        <v>574</v>
       </c>
       <c r="J191" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K191" s="4">
-        <v>2.5316000000000002E-2</v>
+        <v>4.0506E-2</v>
       </c>
       <c r="L191" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M191" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
     </row>
     <row r="192" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10332,7 +10331,7 @@
         <v>14</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>26</v>
@@ -10350,16 +10349,16 @@
         <v>578</v>
       </c>
       <c r="J192" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K192" s="4">
-        <v>4.0506E-2</v>
+        <v>8.1013000000000002E-2</v>
       </c>
       <c r="L192" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M192" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="193" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10373,34 +10372,34 @@
         <v>14</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F193" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="G193" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="G193" s="1" t="s">
+      <c r="H193" s="3">
+        <v>0</v>
+      </c>
+      <c r="I193" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="H193" s="3">
-        <v>0</v>
-      </c>
-      <c r="I193" s="2" t="s">
-        <v>582</v>
-      </c>
       <c r="J193" s="3">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="K193" s="4">
-        <v>8.1013000000000002E-2</v>
+        <v>2.5316000000000002E-2</v>
       </c>
       <c r="L193" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M193" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="194" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10414,34 +10413,34 @@
         <v>14</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="F194" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="H194" s="3">
+        <v>0</v>
+      </c>
+      <c r="I194" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="G194" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="H194" s="3">
-        <v>0</v>
-      </c>
-      <c r="I194" s="2" t="s">
-        <v>585</v>
-      </c>
       <c r="J194" s="3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="K194" s="4">
-        <v>2.5316000000000002E-2</v>
+        <v>6.5823000000000007E-2</v>
       </c>
       <c r="L194" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M194" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10455,37 +10454,37 @@
         <v>14</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>463</v>
+        <v>584</v>
       </c>
       <c r="G195" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="H195" s="3">
+        <v>0</v>
+      </c>
+      <c r="I195" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="H195" s="3">
-        <v>0</v>
-      </c>
-      <c r="I195" s="2" t="s">
-        <v>587</v>
-      </c>
       <c r="J195" s="3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K195" s="4">
-        <v>6.5823000000000007E-2</v>
+        <v>5.0632999999999997E-2</v>
       </c>
       <c r="L195" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M195" s="1" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="196" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>13</v>
       </c>
@@ -10496,37 +10495,37 @@
         <v>14</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F196" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="G196" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="G196" s="1" t="s">
+      <c r="H196" s="3">
+        <v>0</v>
+      </c>
+      <c r="I196" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="H196" s="3">
-        <v>0</v>
-      </c>
-      <c r="I196" s="2" t="s">
+      <c r="J196" s="3">
+        <v>26</v>
+      </c>
+      <c r="K196" s="4">
+        <v>0.13164600000000001</v>
+      </c>
+      <c r="L196" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M196" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="J196" s="3">
-        <v>10</v>
-      </c>
-      <c r="K196" s="4">
-        <v>5.0632999999999997E-2</v>
-      </c>
-      <c r="L196" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M196" s="1" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="197" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>13</v>
       </c>
@@ -10537,7 +10536,7 @@
         <v>14</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>89</v>
@@ -10552,19 +10551,19 @@
         <v>0</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>593</v>
+        <v>522</v>
       </c>
       <c r="J197" s="3">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="K197" s="4">
-        <v>0.13164600000000001</v>
+        <v>5.0632999999999997E-2</v>
       </c>
       <c r="L197" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M197" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="198" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10578,16 +10577,16 @@
         <v>14</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H198" s="3">
         <v>0</v>
@@ -10596,16 +10595,16 @@
         <v>526</v>
       </c>
       <c r="J198" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K198" s="4">
-        <v>5.0632999999999997E-2</v>
+        <v>5.5696000000000002E-2</v>
       </c>
       <c r="L198" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M198" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10619,22 +10618,22 @@
         <v>14</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F199" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="H199" s="3">
+        <v>0</v>
+      </c>
+      <c r="I199" s="2" t="s">
         <v>597</v>
-      </c>
-      <c r="G199" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="H199" s="3">
-        <v>0</v>
-      </c>
-      <c r="I199" s="2" t="s">
-        <v>530</v>
       </c>
       <c r="J199" s="3">
         <v>11</v>
@@ -10646,7 +10645,7 @@
         <v>20</v>
       </c>
       <c r="M199" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="200" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10660,34 +10659,34 @@
         <v>14</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F200" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="G200" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="G200" s="1" t="s">
+      <c r="H200" s="3">
+        <v>0</v>
+      </c>
+      <c r="I200" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="H200" s="3">
-        <v>0</v>
-      </c>
-      <c r="I200" s="2" t="s">
-        <v>601</v>
-      </c>
       <c r="J200" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K200" s="4">
-        <v>5.5696000000000002E-2</v>
+        <v>4.0506E-2</v>
       </c>
       <c r="L200" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M200" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="201" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10701,34 +10700,34 @@
         <v>14</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F201" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="G201" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="G201" s="1" t="s">
+      <c r="H201" s="3">
+        <v>0</v>
+      </c>
+      <c r="I201" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="H201" s="3">
-        <v>0</v>
-      </c>
-      <c r="I201" s="2" t="s">
-        <v>604</v>
-      </c>
       <c r="J201" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K201" s="4">
-        <v>4.0506E-2</v>
+        <v>4.5569999999999999E-2</v>
       </c>
       <c r="L201" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M201" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10742,22 +10741,22 @@
         <v>14</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F202" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="G202" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="G202" s="1" t="s">
+      <c r="H202" s="3">
+        <v>0</v>
+      </c>
+      <c r="I202" s="2" t="s">
         <v>606</v>
-      </c>
-      <c r="H202" s="3">
-        <v>0</v>
-      </c>
-      <c r="I202" s="2" t="s">
-        <v>607</v>
       </c>
       <c r="J202" s="3">
         <v>9</v>
@@ -10769,7 +10768,7 @@
         <v>20</v>
       </c>
       <c r="M202" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="203" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10783,34 +10782,34 @@
         <v>14</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>89</v>
+        <v>324</v>
       </c>
       <c r="F203" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="G203" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="G203" s="1" t="s">
+      <c r="H203" s="3">
+        <v>0</v>
+      </c>
+      <c r="I203" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="H203" s="3">
-        <v>0</v>
-      </c>
-      <c r="I203" s="2" t="s">
-        <v>610</v>
-      </c>
       <c r="J203" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K203" s="4">
-        <v>4.5569999999999999E-2</v>
+        <v>3.5443000000000002E-2</v>
       </c>
       <c r="L203" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M203" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="204" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10824,34 +10823,34 @@
         <v>14</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>324</v>
+        <v>44</v>
       </c>
       <c r="F204" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="G204" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="G204" s="1" t="s">
+      <c r="H204" s="3">
+        <v>0</v>
+      </c>
+      <c r="I204" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="H204" s="3">
-        <v>0</v>
-      </c>
-      <c r="I204" s="2" t="s">
-        <v>613</v>
-      </c>
       <c r="J204" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K204" s="4">
-        <v>3.5443000000000002E-2</v>
+        <v>4.5569999999999999E-2</v>
       </c>
       <c r="L204" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M204" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10865,13 +10864,13 @@
         <v>14</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>554</v>
+        <v>613</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>44</v>
+        <v>614</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>614</v>
+        <v>68</v>
       </c>
       <c r="G205" s="1" t="s">
         <v>615</v>
@@ -10883,16 +10882,16 @@
         <v>616</v>
       </c>
       <c r="J205" s="3">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K205" s="4">
-        <v>4.5569999999999999E-2</v>
+        <v>0.99601600000000001</v>
       </c>
       <c r="L205" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M205" s="1" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
     </row>
     <row r="206" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10906,13 +10905,13 @@
         <v>14</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>617</v>
+        <v>341</v>
       </c>
       <c r="E206" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F206" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>619</v>
@@ -10921,16 +10920,16 @@
         <v>0</v>
       </c>
       <c r="I206" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="J206" s="3">
+        <v>10</v>
+      </c>
+      <c r="K206" s="4">
+        <v>6.7123000000000002E-2</v>
+      </c>
+      <c r="L206" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="J206" s="3">
-        <v>25</v>
-      </c>
-      <c r="K206" s="4">
-        <v>0.99601600000000001</v>
-      </c>
-      <c r="L206" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="M206" s="1" t="s">
         <v>621</v>
@@ -10962,19 +10961,19 @@
         <v>0</v>
       </c>
       <c r="I207" s="2" t="s">
-        <v>416</v>
+        <v>526</v>
       </c>
       <c r="J207" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K207" s="4">
-        <v>6.7123000000000002E-2</v>
+        <v>7.3834999999999998E-2</v>
       </c>
       <c r="L207" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M207" s="1" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="208" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -10991,31 +10990,31 @@
         <v>341</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F208" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="H208" s="3">
+        <v>0</v>
+      </c>
+      <c r="I208" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J208" s="3">
+        <v>5</v>
+      </c>
+      <c r="K208" s="4">
+        <v>3.3562000000000002E-2</v>
+      </c>
+      <c r="L208" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="M208" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="G208" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="H208" s="3">
-        <v>0</v>
-      </c>
-      <c r="I208" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="J208" s="3">
-        <v>11</v>
-      </c>
-      <c r="K208" s="4">
-        <v>7.3834999999999998E-2</v>
-      </c>
-      <c r="L208" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="M208" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="209" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -11029,31 +11028,31 @@
         <v>14</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>341</v>
+        <v>71</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="F209" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G209" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="G209" s="1" t="s">
+      <c r="H209" s="3">
+        <v>0</v>
+      </c>
+      <c r="I209" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="H209" s="3">
-        <v>0</v>
-      </c>
-      <c r="I209" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="J209" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K209" s="4">
-        <v>3.3562000000000002E-2</v>
+        <v>2.6654000000000001E-2</v>
       </c>
       <c r="L209" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M209" s="1" t="s">
         <v>630</v>
@@ -11070,34 +11069,34 @@
         <v>14</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>71</v>
+        <v>276</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>233</v>
+        <v>631</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H210" s="3">
         <v>0</v>
       </c>
       <c r="I210" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="J210" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K210" s="4">
-        <v>2.6654000000000001E-2</v>
+        <v>4.2592999999999999E-2</v>
       </c>
       <c r="L210" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M210" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -11111,10 +11110,10 @@
         <v>14</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>276</v>
+        <v>497</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>635</v>
+        <v>39</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>636</v>
@@ -11129,13 +11128,13 @@
         <v>638</v>
       </c>
       <c r="J211" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K211" s="4">
-        <v>4.2592999999999999E-2</v>
+        <v>3.6783000000000003E-2</v>
       </c>
       <c r="L211" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M211" s="1" t="s">
         <v>639</v>
@@ -11152,10 +11151,10 @@
         <v>14</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>501</v>
+        <v>71</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>640</v>
@@ -11170,13 +11169,13 @@
         <v>642</v>
       </c>
       <c r="J212" s="3">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="K212" s="4">
-        <v>3.6783000000000003E-2</v>
+        <v>0.14659800000000001</v>
       </c>
       <c r="L212" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M212" s="1" t="s">
         <v>643</v>
@@ -11193,7 +11192,7 @@
         <v>14</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>44</v>
@@ -11211,19 +11210,19 @@
         <v>646</v>
       </c>
       <c r="J213" s="3">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K213" s="4">
-        <v>0.14659800000000001</v>
+        <v>5.7685E-2</v>
       </c>
       <c r="L213" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M213" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
         <v>13</v>
       </c>
@@ -11234,7 +11233,7 @@
         <v>14</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>167</v>
+        <v>380</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>44</v>
@@ -11252,19 +11251,19 @@
         <v>650</v>
       </c>
       <c r="J214" s="3">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K214" s="4">
-        <v>5.7685E-2</v>
+        <v>0.138881</v>
       </c>
       <c r="L214" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M214" s="1" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="215" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
         <v>13</v>
       </c>
@@ -11275,37 +11274,37 @@
         <v>14</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F215" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="G215" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="G215" s="1" t="s">
+      <c r="H215" s="3">
+        <v>0</v>
+      </c>
+      <c r="I215" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="H215" s="3">
-        <v>0</v>
-      </c>
-      <c r="I215" s="2" t="s">
+      <c r="J215" s="3">
+        <v>19</v>
+      </c>
+      <c r="K215" s="4">
+        <v>0.12753400000000001</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="M215" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="J215" s="3">
-        <v>23</v>
-      </c>
-      <c r="K215" s="4">
-        <v>0.138881</v>
-      </c>
-      <c r="L215" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="M215" s="1" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="216" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>13</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>14</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>341</v>
+        <v>380</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>44</v>
@@ -11334,13 +11333,13 @@
         <v>657</v>
       </c>
       <c r="J216" s="3">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="K216" s="4">
-        <v>0.12753400000000001</v>
+        <v>0.14491899999999999</v>
       </c>
       <c r="L216" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="M216" s="1" t="s">
         <v>658</v>

</xml_diff>